<commit_message>
For optimization, we are nopw attempting to just use pyzbar to identify the barcode and if this fails we then go to the CNN for further analysis.
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasondank/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasondank/PycharmProjects/BarcodeSodexoV1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E02B295-4473-6D49-9C2F-518507672A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F8A3DB-FCC8-504F-AE60-F9C6387AB57F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" xr2:uid="{7D3B42C4-B5DF-2E42-AAF0-4AEBB6C9C24B}"/>
+    <workbookView xWindow="5180" yWindow="2580" windowWidth="28040" windowHeight="17440" xr2:uid="{7D3B42C4-B5DF-2E42-AAF0-4AEBB6C9C24B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>ItemNumber</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>Water</t>
+  </si>
+  <si>
+    <t>Hotdog Bun</t>
+  </si>
+  <si>
+    <t>Hamburger Bun</t>
   </si>
 </sst>
 </file>
@@ -451,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A8ACAF-CDEC-FB49-90C1-DABB10AE0426}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -563,6 +569,28 @@
         <v>2.98</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>968149</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>966705</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>1.23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>